<commit_message>
Make updates so it can run from no memory (I ran on new computer)
</commit_message>
<xml_diff>
--- a/Data/Research Data Master List.xlsx
+++ b/Data/Research Data Master List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonntag\Github\EvapCoolerUtahCounty\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0EFE07-9721-4AE8-8CA3-C1C7AD9C76EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50889289-76D8-497E-ABCD-0B7E40E8264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="2115" windowWidth="17490" windowHeight="14250" activeTab="2" xr2:uid="{AC9A91AC-7678-4C7F-8916-15799EFE6E2D}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{AC9A91AC-7678-4C7F-8916-15799EFE6E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Visit" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="302">
   <si>
     <t>House.Number</t>
   </si>
@@ -762,12 +762,6 @@
   </si>
   <si>
     <t>Indoor SidePak is much larger than indoor. Outdoor SidePak ends prematurely</t>
-  </si>
-  <si>
-    <t>Temp notes</t>
-  </si>
-  <si>
-    <t>RH notes</t>
   </si>
   <si>
     <t>What type of furnance filters fo you typically purchase?</t>
@@ -1518,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F2A8AE-F84B-4894-B6A1-E396CF2340C1}">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1537,7 +1531,7 @@
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1565,14 +1559,8 @@
       <c r="I1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1602,7 +1590,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1632,7 +1620,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1658,7 +1646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1684,7 +1672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -1714,7 +1702,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -1741,7 +1729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1767,7 +1755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1795,7 +1783,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -1821,7 +1809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -1849,7 +1837,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1875,7 +1863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -1901,7 +1889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1929,7 +1917,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -1955,7 +1943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -3576,7 +3564,7 @@
     </row>
     <row r="2" spans="1:26" ht="13.5" thickBot="1">
       <c r="A2" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>187</v>
@@ -3610,7 +3598,7 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1">
       <c r="A3" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>189</v>
@@ -3644,7 +3632,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
       <c r="A4" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>190</v>
@@ -3678,7 +3666,7 @@
     </row>
     <row r="5" spans="1:26" ht="18" customHeight="1" thickBot="1">
       <c r="A5" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>191</v>
@@ -3712,7 +3700,7 @@
     </row>
     <row r="6" spans="1:26" ht="13.5" thickBot="1">
       <c r="A6" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>192</v>
@@ -3746,7 +3734,7 @@
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" thickBot="1">
       <c r="A7" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>193</v>
@@ -3780,7 +3768,7 @@
     </row>
     <row r="8" spans="1:26" ht="13.5" thickBot="1">
       <c r="A8" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>194</v>
@@ -3814,7 +3802,7 @@
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1">
       <c r="A9" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>195</v>
@@ -3848,7 +3836,7 @@
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1">
       <c r="A10" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>196</v>
@@ -3882,7 +3870,7 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1">
       <c r="A11" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>197</v>
@@ -3916,7 +3904,7 @@
     </row>
     <row r="12" spans="1:26" ht="13.5" thickBot="1">
       <c r="A12" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>198</v>
@@ -3947,7 +3935,7 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" thickBot="1">
       <c r="A13" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>199</v>
@@ -3979,7 +3967,7 @@
     </row>
     <row r="14" spans="1:26" ht="13.5" thickBot="1">
       <c r="A14" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>200</v>
@@ -4011,7 +3999,7 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" thickBot="1">
       <c r="A15" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>201</v>
@@ -4043,7 +4031,7 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" thickBot="1">
       <c r="A16" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>202</v>
@@ -4075,7 +4063,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" thickBot="1">
       <c r="A17" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>203</v>
@@ -4107,7 +4095,7 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" thickBot="1">
       <c r="A18" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>204</v>
@@ -4139,7 +4127,7 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" thickBot="1">
       <c r="A19" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>205</v>
@@ -4171,7 +4159,7 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" thickBot="1">
       <c r="A20" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>206</v>
@@ -4203,7 +4191,7 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" thickBot="1">
       <c r="A21" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>207</v>
@@ -4235,7 +4223,7 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" thickBot="1">
       <c r="A22" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>208</v>
@@ -4267,7 +4255,7 @@
     </row>
     <row r="23" spans="1:26" ht="26.25" thickBot="1">
       <c r="A23" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>209</v>
@@ -4299,7 +4287,7 @@
     </row>
     <row r="24" spans="1:26" ht="13.5" thickBot="1">
       <c r="A24" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>210</v>
@@ -4331,7 +4319,7 @@
     </row>
     <row r="25" spans="1:26" ht="13.5" thickBot="1">
       <c r="A25" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>211</v>
@@ -4363,7 +4351,7 @@
     </row>
     <row r="26" spans="1:26" ht="13.5" thickBot="1">
       <c r="A26" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>212</v>
@@ -4395,7 +4383,7 @@
     </row>
     <row r="27" spans="1:26" ht="13.5" thickBot="1">
       <c r="A27" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>213</v>
@@ -4427,7 +4415,7 @@
     </row>
     <row r="28" spans="1:26" ht="13.5" thickBot="1">
       <c r="A28" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>214</v>
@@ -4459,7 +4447,7 @@
     </row>
     <row r="29" spans="1:26" ht="26.25" thickBot="1">
       <c r="A29" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>215</v>
@@ -4491,10 +4479,10 @@
     </row>
     <row r="30" spans="1:26" ht="13.5" thickBot="1">
       <c r="A30" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="16"/>
@@ -4524,19 +4512,19 @@
     <row r="31" spans="1:26">
       <c r="A31" s="19"/>
       <c r="B31" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:26">
       <c r="A32" s="19"/>
       <c r="B32" s="22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="19"/>
       <c r="B33" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4547,28 +4535,28 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="19"/>
       <c r="B36" s="22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="19"/>
       <c r="B37" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="19"/>
       <c r="B38" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4588,7 +4576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDBF968-4651-4D4E-AB3F-92041501F8CD}">
   <dimension ref="A1:AH85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH30" sqref="AH30"/>
     </sheetView>
   </sheetViews>
@@ -6592,7 +6580,7 @@
         <v>111</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:34">
@@ -7477,7 +7465,7 @@
         <v>105</v>
       </c>
       <c r="AH29" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:34">
@@ -8686,7 +8674,7 @@
         <v>37</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -9031,7 +9019,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>37</v>
@@ -9048,7 +9036,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>37</v>
@@ -9063,15 +9051,15 @@
         <v>37</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>37</v>
@@ -9088,7 +9076,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>48</v>
@@ -9105,7 +9093,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>37</v>
@@ -9122,7 +9110,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>37</v>
@@ -9139,7 +9127,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>37</v>
@@ -9156,7 +9144,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>37</v>
@@ -9171,15 +9159,15 @@
         <v>37</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>38</v>
@@ -9196,7 +9184,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>38</v>
@@ -9211,12 +9199,12 @@
         <v>37</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>48</v>
@@ -9233,7 +9221,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>37</v>
@@ -9250,7 +9238,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>37</v>
@@ -9267,7 +9255,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>48</v>
@@ -9284,7 +9272,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>38</v>
@@ -9301,7 +9289,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>37</v>
@@ -9318,7 +9306,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>37</v>
@@ -9335,7 +9323,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>38</v>
@@ -9352,7 +9340,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>48</v>
@@ -9369,7 +9357,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>38</v>
@@ -9386,7 +9374,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>38</v>
@@ -9403,7 +9391,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>38</v>
@@ -9420,7 +9408,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>38</v>
@@ -9437,7 +9425,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>38</v>
@@ -9454,7 +9442,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>38</v>
@@ -9471,7 +9459,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>38</v>
@@ -9488,7 +9476,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>38</v>
@@ -9505,7 +9493,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>38</v>

</xml_diff>